<commit_message>
building a leaflet map
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PRJ\StateRx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3994CDA-4DE0-44A6-88CF-2FCFAF5023D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C02704-B871-4B25-9246-E92049420853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{25158DE5-819B-4E9C-8133-8EC91A336281}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <sheet name="documentation" sheetId="10" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">checklist!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">checklist!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,24 +56,14 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={776A275C-758D-471B-847E-58C6569DED9A}</author>
     <author>tc={C280DFDA-8842-4B1C-AE96-72B86856422E}</author>
-    <author>tc={D7D38920-818F-42B5-94B0-7A8CD97CEE28}</author>
     <author>tc={65EDE810-8AD2-40CE-B77D-4D2EDE09ADBA}</author>
     <author>tc={B8BAA343-7DCC-41E7-8F12-49892F436CCB}</author>
     <author>tc={8CE3DA89-5276-402C-868B-7B009D28D41A}</author>
     <author>tc={5BA2D2E3-E62E-4405-A605-5A743B906387}</author>
   </authors>
   <commentList>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{776A275C-758D-471B-847E-58C6569DED9A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    These are acres requested daily and may not reflect the total acreage that was intended to be burned</t>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="1" shapeId="0" xr:uid="{C280DFDA-8842-4B1C-AE96-72B86856422E}">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{C280DFDA-8842-4B1C-AE96-72B86856422E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -81,15 +71,7 @@
     I was unable to figure out the permits so I don't have this info for UT</t>
       </text>
     </comment>
-    <comment ref="E5" authorId="2" shapeId="0" xr:uid="{D7D38920-818F-42B5-94B0-7A8CD97CEE28}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    These are acres proposed on a daily basis; there are no permitted acres</t>
-      </text>
-    </comment>
-    <comment ref="E7" authorId="3" shapeId="0" xr:uid="{65EDE810-8AD2-40CE-B77D-4D2EDE09ADBA}">
+    <comment ref="F7" authorId="1" shapeId="0" xr:uid="{65EDE810-8AD2-40CE-B77D-4D2EDE09ADBA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -97,7 +79,7 @@
     I did not process but I could try</t>
       </text>
     </comment>
-    <comment ref="B10" authorId="4" shapeId="0" xr:uid="{B8BAA343-7DCC-41E7-8F12-49892F436CCB}">
+    <comment ref="B10" authorId="2" shapeId="0" xr:uid="{B8BAA343-7DCC-41E7-8F12-49892F436CCB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -105,7 +87,7 @@
     Not sure how to find unique burns, emailed contact</t>
       </text>
     </comment>
-    <comment ref="A11" authorId="5" shapeId="0" xr:uid="{8CE3DA89-5276-402C-868B-7B009D28D41A}">
+    <comment ref="A11" authorId="3" shapeId="0" xr:uid="{8CE3DA89-5276-402C-868B-7B009D28D41A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -113,7 +95,7 @@
     Hold off until new data is provided</t>
       </text>
     </comment>
-    <comment ref="A12" authorId="6" shapeId="0" xr:uid="{5BA2D2E3-E62E-4405-A605-5A743B906387}">
+    <comment ref="A12" authorId="4" shapeId="0" xr:uid="{5BA2D2E3-E62E-4405-A605-5A743B906387}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -126,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="203">
   <si>
     <t>after data are compiled draft check of the data to find and fix errors</t>
   </si>
@@ -542,9 +524,6 @@
     <t>ID, consider limiting data to 2013 to present when data collection was most consistent</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>appears to have multipel requests, but the permited acres for the same request in the same year can change</t>
   </si>
   <si>
@@ -560,9 +539,6 @@
     <t>remove dup rows in raw dataset?</t>
   </si>
   <si>
-    <t>check number of rows w/ read_csv vs. origional</t>
-  </si>
-  <si>
     <t>TO DO</t>
   </si>
   <si>
@@ -602,9 +578,6 @@
     <t>20 acres completed over 2 days? Or 10 acres total?</t>
   </si>
   <si>
-    <t>PERMIT</t>
-  </si>
-  <si>
     <t>COMPLETE</t>
   </si>
   <si>
@@ -638,13 +611,7 @@
     <t>asked Jason about how to calc permited and accomplished when there are multiple requests</t>
   </si>
   <si>
-    <t>no, no permit numbers used; probably need to use burn names and location</t>
-  </si>
-  <si>
     <t>it looks like proposed acres is updated daily and could be changed based on previous day's request so summing them may not give the planned acres. Might just get completed?</t>
-  </si>
-  <si>
-    <t>get distinct rows</t>
   </si>
   <si>
     <t>consider adding "Prescribed Fire" to the list of broadcast burn words for classifying burn type</t>
@@ -775,6 +742,18 @@
   </si>
   <si>
     <t>source id, burn name, lat, lon</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>get distinct rows pre-process (no duplicate records)</t>
+  </si>
+  <si>
+    <t>REQUEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PERMIT </t>
   </si>
 </sst>
 </file>
@@ -833,7 +812,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -861,12 +840,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -918,18 +891,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -966,7 +927,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -974,30 +934,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1969,16 +1936,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E2" dT="2023-11-13T20:35:25.64" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{776A275C-758D-471B-847E-58C6569DED9A}">
-    <text>These are acres requested daily and may not reflect the total acreage that was intended to be burned</text>
-  </threadedComment>
-  <threadedComment ref="E3" dT="2023-11-13T14:16:34.31" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{C280DFDA-8842-4B1C-AE96-72B86856422E}">
+  <threadedComment ref="F3" dT="2023-11-13T14:16:34.31" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{C280DFDA-8842-4B1C-AE96-72B86856422E}">
     <text>I was unable to figure out the permits so I don't have this info for UT</text>
   </threadedComment>
-  <threadedComment ref="E5" dT="2023-11-13T20:34:42.34" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{D7D38920-818F-42B5-94B0-7A8CD97CEE28}">
-    <text>These are acres proposed on a daily basis; there are no permitted acres</text>
-  </threadedComment>
-  <threadedComment ref="E7" dT="2023-11-13T14:09:22.92" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{65EDE810-8AD2-40CE-B77D-4D2EDE09ADBA}">
+  <threadedComment ref="F7" dT="2023-11-13T14:09:22.92" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{65EDE810-8AD2-40CE-B77D-4D2EDE09ADBA}">
     <text>I did not process but I could try</text>
   </threadedComment>
   <threadedComment ref="B10" dT="2023-11-09T17:46:37.50" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{B8BAA343-7DCC-41E7-8F12-49892F436CCB}">
@@ -2005,12 +1966,12 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2028,7 +1989,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="27"/>
+    <col min="1" max="1" width="8.88671875" style="26"/>
     <col min="2" max="2" width="103.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2036,103 +1997,103 @@
       <c r="A1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>193</v>
+      <c r="B1" s="27" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="C7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="19" t="s">
+    <row r="8" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>188</v>
-      </c>
-      <c r="C7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>187</v>
-      </c>
-      <c r="C8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="C9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>194</v>
-      </c>
     </row>
     <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>186</v>
+      <c r="B11" s="30" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2508,10 +2469,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0118C388-E1CB-44F3-ACC3-F76C30052EB0}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2519,33 +2480,33 @@
     <col min="2" max="2" width="17.77734375" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.88671875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="58.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="58.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
         <v>67</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>162</v>
+      <c r="C1" s="16" t="s">
+        <v>159</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>104</v>
+        <v>193</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>156</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>113</v>
@@ -2556,38 +2517,35 @@
       <c r="J1" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="L1" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="9" t="s">
+      <c r="K1" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="M1" s="10"/>
+      <c r="N1" s="9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>170</v>
+        <v>133</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>175</v>
+        <v>44</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>44</v>
+        <v>133</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>44</v>
@@ -2601,29 +2559,31 @@
       <c r="J2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="9" t="s">
+      <c r="K2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="C3" s="10"/>
+      <c r="B3" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>133</v>
+      </c>
       <c r="D3" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>133</v>
+        <v>196</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>44</v>
@@ -2637,20 +2597,17 @@
       <c r="J3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="K3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="O3" s="9" t="s">
+      <c r="K3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="N3" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>94</v>
       </c>
@@ -2658,13 +2615,10 @@
         <v>133</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>44</v>
+        <v>160</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>195</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>44</v>
@@ -2681,29 +2635,27 @@
       <c r="J4" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K4" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>176</v>
+      <c r="B5" s="33" t="s">
+        <v>171</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="35" t="s">
-        <v>200</v>
+      <c r="D5" s="10" t="s">
+        <v>195</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F5" s="3"/>
       <c r="G5" s="10" t="s">
-        <v>138</v>
+        <v>44</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>44</v>
@@ -2714,14 +2666,14 @@
       <c r="J5" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="L5" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="O5" s="9" t="s">
+      <c r="K5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>97</v>
       </c>
@@ -2729,13 +2681,10 @@
         <v>133</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>44</v>
+        <v>160</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>195</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>44</v>
@@ -2752,35 +2701,29 @@
       <c r="J6" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="K6" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" t="s">
-        <v>146</v>
-      </c>
-      <c r="O6" s="9" t="s">
+      <c r="K6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" t="s">
+        <v>144</v>
+      </c>
+      <c r="N6" s="9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>180</v>
+      <c r="B7" s="33" t="s">
+        <v>175</v>
       </c>
       <c r="C7" s="10"/>
-      <c r="D7" s="35" t="s">
-        <v>200</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>133</v>
+      <c r="D7" s="10" t="s">
+        <v>195</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>44</v>
@@ -2792,31 +2735,28 @@
         <v>44</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M7" t="s">
-        <v>154</v>
-      </c>
-      <c r="O7" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" t="s">
+        <v>152</v>
+      </c>
+      <c r="N7" s="9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>183</v>
+      <c r="B8" s="33" t="s">
+        <v>178</v>
       </c>
       <c r="C8" s="10"/>
-      <c r="D8" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>44</v>
+      <c r="D8" s="10" t="s">
+        <v>195</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>44</v>
@@ -2833,14 +2773,14 @@
       <c r="J8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="L8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M8" s="19" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>102</v>
       </c>
@@ -2848,13 +2788,10 @@
         <v>133</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>44</v>
+        <v>198</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>44</v>
@@ -2871,26 +2808,23 @@
       <c r="J9" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="L9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M9" s="10"/>
-      <c r="O9" s="9" t="s">
+      <c r="K9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="10"/>
+      <c r="N9" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>92</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>44</v>
+      <c r="C10" s="33" t="s">
+        <v>162</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>44</v>
@@ -2907,29 +2841,26 @@
       <c r="J10" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="L10" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+      <c r="K10" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="E11" s="10" t="s">
-        <v>44</v>
-      </c>
+      <c r="C11" s="17"/>
       <c r="F11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>127</v>
-      </c>
       <c r="H11" s="10" t="s">
-        <v>44</v>
+        <v>199</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>127</v>
@@ -2937,30 +2868,28 @@
       <c r="J11" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K11" s="3"/>
+      <c r="L11" s="17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>179</v>
+      <c r="B12" s="34" t="s">
+        <v>174</v>
       </c>
       <c r="C12" s="10"/>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>44</v>
+      <c r="H12" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>44</v>
@@ -2971,92 +2900,89 @@
       <c r="K12" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="L12" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="M13" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L13" s="20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="16"/>
-      <c r="E15" s="14"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="14"/>
-      <c r="O15" s="9" t="s">
+      <c r="G15" s="14"/>
+      <c r="N15" s="9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O16" s="9" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N16" s="9" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
-      <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="O17" s="9" t="s">
+      <c r="N17" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
-      <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="O19" s="13" t="s">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N19" s="13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="O20" s="13" t="s">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N20" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N23" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="O22" t="s">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N24" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="O23" t="s">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N25" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="O24" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="O25" t="s">
-        <v>151</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{0118C388-E1CB-44F3-ACC3-F76C30052EB0}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M13">
+  <autoFilter ref="A1:L1" xr:uid="{0118C388-E1CB-44F3-ACC3-F76C30052EB0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L13">
       <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>
@@ -3171,7 +3097,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C14" s="15"/>
     </row>
@@ -3337,12 +3263,12 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -3363,17 +3289,17 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3393,28 +3319,28 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>171</v>
+      <c r="A1" s="21" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3505,27 +3431,27 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>169</v>
+      <c r="B3" s="22" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>177</v>
+      <c r="B4" s="22" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>181</v>
+      <c r="B5" s="25" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3533,7 +3459,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3541,7 +3467,7 @@
         <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3597,7 +3523,7 @@
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O10" s="1"/>
     </row>
@@ -3714,12 +3640,12 @@
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.3">
@@ -3729,12 +3655,12 @@
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to distinguish permitted, requested, and accomplished
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PRJ\StateRx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C02704-B871-4B25-9246-E92049420853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B660E4B0-5978-44F1-8BFC-A58BE7175648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{25158DE5-819B-4E9C-8133-8EC91A336281}"/>
   </bookViews>
@@ -56,14 +56,23 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={E3B74EA3-F325-4812-AD83-C5D6415668FF}</author>
     <author>tc={C280DFDA-8842-4B1C-AE96-72B86856422E}</author>
+    <author>tc={06B7A9A7-A445-4252-9CCB-57D3686DFA02}</author>
     <author>tc={65EDE810-8AD2-40CE-B77D-4D2EDE09ADBA}</author>
-    <author>tc={B8BAA343-7DCC-41E7-8F12-49892F436CCB}</author>
+    <author>tc={D1A9D9B6-E17A-4DCC-A6A1-F9EB8CAC74A1}</author>
     <author>tc={8CE3DA89-5276-402C-868B-7B009D28D41A}</author>
-    <author>tc={5BA2D2E3-E62E-4405-A605-5A743B906387}</author>
   </authors>
   <commentList>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{C280DFDA-8842-4B1C-AE96-72B86856422E}">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{E3B74EA3-F325-4812-AD83-C5D6415668FF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    There are requests, but I dropped some of them at the beginning of the r script; go back and check if this is what I want to do; for now data are for completed requests</t>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="1" shapeId="0" xr:uid="{C280DFDA-8842-4B1C-AE96-72B86856422E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -71,7 +80,15 @@
     I was unable to figure out the permits so I don't have this info for UT</t>
       </text>
     </comment>
-    <comment ref="F7" authorId="1" shapeId="0" xr:uid="{65EDE810-8AD2-40CE-B77D-4D2EDE09ADBA}">
+    <comment ref="E7" authorId="2" shapeId="0" xr:uid="{06B7A9A7-A445-4252-9CCB-57D3686DFA02}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I'm working from the accomplished spreadsheet so I don't think I should say anything about requests b/c presumably I only have requests that were accomplished</t>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="3" shapeId="0" xr:uid="{65EDE810-8AD2-40CE-B77D-4D2EDE09ADBA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -79,15 +96,16 @@
     I did not process but I could try</t>
       </text>
     </comment>
-    <comment ref="B10" authorId="2" shapeId="0" xr:uid="{B8BAA343-7DCC-41E7-8F12-49892F436CCB}">
+    <comment ref="E10" authorId="4" shapeId="0" xr:uid="{D1A9D9B6-E17A-4DCC-A6A1-F9EB8CAC74A1}">
       <text>
-        <t>[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Not sure how to find unique burns, emailed contact</t>
+    Requested acres: can put in a big number so they are not boxed in; Matt doesn’t recommend using requests
+</t>
       </text>
     </comment>
-    <comment ref="A11" authorId="3" shapeId="0" xr:uid="{8CE3DA89-5276-402C-868B-7B009D28D41A}">
+    <comment ref="A11" authorId="5" shapeId="0" xr:uid="{8CE3DA89-5276-402C-868B-7B009D28D41A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -95,20 +113,12 @@
     Hold off until new data is provided</t>
       </text>
     </comment>
-    <comment ref="A12" authorId="4" shapeId="0" xr:uid="{5BA2D2E3-E62E-4405-A605-5A743B906387}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Unclear about data received; wait for email response before processing</t>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="206">
   <si>
     <t>after data are compiled draft check of the data to find and fix errors</t>
   </si>
@@ -630,9 +640,6 @@
   </si>
   <si>
     <t>need to separate by burn type</t>
-  </si>
-  <si>
-    <t>yes, pretty sure I can sum completed to get accomplished, but account for burn type, sent email to contact</t>
   </si>
   <si>
     <t>yes, pretty sure I can sum completed to get accomplished, sent email to contact</t>
@@ -755,12 +762,43 @@
   <si>
     <t xml:space="preserve">PERMIT </t>
   </si>
+  <si>
+    <t>source id, lat, lon</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>washoe and clark county requests</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; update script formatting based on new style</t>
+    </r>
+  </si>
+  <si>
+    <t>TONS</t>
+  </si>
+  <si>
+    <t>standardize, sometimes planned, sometimes completed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -810,6 +848,12 @@
       <color rgb="FFDE935F"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -904,7 +948,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -937,7 +981,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -953,18 +996,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="fill"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1936,20 +1977,24 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E3" dT="2023-11-17T22:35:18.89" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{E3B74EA3-F325-4812-AD83-C5D6415668FF}">
+    <text>There are requests, but I dropped some of them at the beginning of the r script; go back and check if this is what I want to do; for now data are for completed requests</text>
+  </threadedComment>
   <threadedComment ref="F3" dT="2023-11-13T14:16:34.31" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{C280DFDA-8842-4B1C-AE96-72B86856422E}">
     <text>I was unable to figure out the permits so I don't have this info for UT</text>
+  </threadedComment>
+  <threadedComment ref="E7" dT="2023-11-17T21:41:26.54" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{06B7A9A7-A445-4252-9CCB-57D3686DFA02}">
+    <text>I'm working from the accomplished spreadsheet so I don't think I should say anything about requests b/c presumably I only have requests that were accomplished</text>
   </threadedComment>
   <threadedComment ref="F7" dT="2023-11-13T14:09:22.92" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{65EDE810-8AD2-40CE-B77D-4D2EDE09ADBA}">
     <text>I did not process but I could try</text>
   </threadedComment>
-  <threadedComment ref="B10" dT="2023-11-09T17:46:37.50" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{B8BAA343-7DCC-41E7-8F12-49892F436CCB}">
-    <text>Not sure how to find unique burns, emailed contact</text>
+  <threadedComment ref="E10" dT="2023-11-17T19:41:07.47" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{D1A9D9B6-E17A-4DCC-A6A1-F9EB8CAC74A1}">
+    <text xml:space="preserve">Requested acres: can put in a big number so they are not boxed in; Matt doesn’t recommend using requests
+</text>
   </threadedComment>
   <threadedComment ref="A11" dT="2023-11-13T20:20:25.03" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{8CE3DA89-5276-402C-868B-7B009D28D41A}">
     <text>Hold off until new data is provided</text>
-  </threadedComment>
-  <threadedComment ref="A12" dT="2023-11-15T23:59:18.92" personId="{36267AC1-CAE9-4E6F-905C-D1D9763ABC5D}" id="{5BA2D2E3-E62E-4405-A605-5A743B906387}">
-    <text>Unclear about data received; wait for email response before processing</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1989,7 +2034,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="26"/>
+    <col min="1" max="1" width="8.88671875" style="25"/>
     <col min="2" max="2" width="103.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1997,31 +2042,31 @@
       <c r="A1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="27" t="s">
-        <v>188</v>
+      <c r="B1" s="26" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>187</v>
+      <c r="B2" s="26" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>95</v>
       </c>
       <c r="B4" t="s">
@@ -2029,71 +2074,71 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>185</v>
+      <c r="B5" s="27" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>97</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C6" s="14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="C7" t="s">
-        <v>192</v>
-      </c>
-    </row>
     <row r="8" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="29" t="s">
-        <v>182</v>
+      <c r="B8" s="28" t="s">
+        <v>181</v>
       </c>
       <c r="C8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="29" t="s">
         <v>180</v>
-      </c>
-      <c r="C9" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2160,14 +2205,14 @@
       <c r="A1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="32"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
@@ -2472,7 +2517,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2487,7 +2532,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>67</v>
       </c>
       <c r="B1" s="10" t="s">
@@ -2497,13 +2542,13 @@
         <v>159</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E1" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>201</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>202</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>156</v>
@@ -2518,7 +2563,7 @@
         <v>126</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>143</v>
@@ -2529,7 +2574,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="21" t="s">
         <v>93</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -2539,7 +2584,7 @@
         <v>133</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>44</v>
@@ -2567,20 +2612,20 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>197</v>
+      <c r="B3" s="31" t="s">
+        <v>196</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>133</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>170</v>
@@ -2608,17 +2653,20 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="21" t="s">
         <v>94</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="3" t="s">
         <v>160</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>133</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>44</v>
@@ -2640,20 +2688,22 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="31" t="s">
         <v>171</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="10" t="s">
+        <v>133</v>
+      </c>
       <c r="G5" s="10" t="s">
         <v>44</v>
       </c>
@@ -2674,17 +2724,20 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="21" t="s">
         <v>97</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="3" t="s">
         <v>160</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>133</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>44</v>
@@ -2712,15 +2765,18 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="33" t="s">
-        <v>175</v>
+      <c r="B7" s="31" t="s">
+        <v>174</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>170</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>170</v>
@@ -2748,15 +2804,18 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="33" t="s">
-        <v>178</v>
+      <c r="B8" s="31" t="s">
+        <v>177</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>44</v>
@@ -2777,21 +2836,24 @@
         <v>44</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="21" t="s">
         <v>102</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>133</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>133</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>44</v>
@@ -2817,17 +2879,23 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="21" t="s">
         <v>92</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="31" t="s">
         <v>162</v>
       </c>
+      <c r="D10" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="F10" s="10" t="s">
-        <v>44</v>
+        <v>133</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>44</v>
@@ -2849,59 +2917,68 @@
       <c r="A11" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="32" t="s">
         <v>136</v>
       </c>
       <c r="C11" s="17"/>
-      <c r="F11" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="10" t="s">
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="I11" s="10" t="s">
+      <c r="H11" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="I11" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="K11" s="3"/>
+      <c r="K11" s="17"/>
       <c r="L11" s="17" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="21" t="s">
         <v>98</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="C12" s="10"/>
+        <v>110</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="E12" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="3" t="s">
+      <c r="F12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>199</v>
+      <c r="H12" s="10" t="s">
+        <v>133</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L12" t="s">
-        <v>144</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -2909,7 +2986,7 @@
         <v>30</v>
       </c>
       <c r="L13" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -3447,11 +3524,11 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>176</v>
+      <c r="B5" s="24" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3459,7 +3536,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3467,7 +3544,7 @@
         <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -3477,10 +3554,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C83686E-AC74-4D6B-A4E0-A59B79186090}">
-  <dimension ref="B2:Q44"/>
+  <dimension ref="B2:Q47"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3663,6 +3740,16 @@
         <v>169</v>
       </c>
     </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
limited time period and removed yard waste points
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PRJ\StateRx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B660E4B0-5978-44F1-8BFC-A58BE7175648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD93FF7C-3791-4C9B-9552-74419D405F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{25158DE5-819B-4E9C-8133-8EC91A336281}"/>
+    <workbookView xWindow="3000" yWindow="1308" windowWidth="18660" windowHeight="12372" firstSheet="5" activeTab="10" xr2:uid="{25158DE5-819B-4E9C-8133-8EC91A336281}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="16" r:id="rId1"/>
@@ -22,13 +22,13 @@
     <sheet name="CA" sheetId="9" r:id="rId7"/>
     <sheet name="inquiries" sheetId="8" r:id="rId8"/>
     <sheet name="to do 2" sheetId="2" r:id="rId9"/>
-    <sheet name="burn status" sheetId="17" r:id="rId10"/>
-    <sheet name="to do spatial overlays" sheetId="7" r:id="rId11"/>
-    <sheet name="plots" sheetId="3" r:id="rId12"/>
-    <sheet name="tabular summary" sheetId="6" r:id="rId13"/>
-    <sheet name="spatial summaries" sheetId="4" r:id="rId14"/>
-    <sheet name="maps" sheetId="5" r:id="rId15"/>
-    <sheet name="documentation" sheetId="10" r:id="rId16"/>
+    <sheet name="to do spatial overlays" sheetId="7" r:id="rId10"/>
+    <sheet name="plots" sheetId="3" r:id="rId11"/>
+    <sheet name="tabular summary" sheetId="6" r:id="rId12"/>
+    <sheet name="spatial summaries" sheetId="4" r:id="rId13"/>
+    <sheet name="maps" sheetId="5" r:id="rId14"/>
+    <sheet name="documentation" sheetId="10" r:id="rId15"/>
+    <sheet name="burn status" sheetId="17" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">checklist!$A$1:$L$1</definedName>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="207">
   <si>
     <t>after data are compiled draft check of the data to find and fix errors</t>
   </si>
@@ -613,9 +613,6 @@
   </si>
   <si>
     <t>see email from Kristy</t>
-  </si>
-  <si>
-    <t>workshop plan: explore data for 1 or several states?</t>
   </si>
   <si>
     <t>asked Jason about how to calc permited and accomplished when there are multiple requests</t>
@@ -793,12 +790,18 @@
   <si>
     <t>standardize, sometimes planned, sometimes completed</t>
   </si>
+  <si>
+    <t>how to define unique: used several criteria for the leaflet map the used narrower criteria (just unique lat/lon) for plots</t>
+  </si>
+  <si>
+    <t>I NEED help w/ logic for filtering for unique values; how do I make sure I get the right burn status?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,12 +851,6 @@
       <color rgb="FFDE935F"/>
       <name val="Lucida Console"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1002,10 +999,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2001,10 +1998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8DF838-E91F-479B-BB7E-4DB4DA2419B3}">
-  <dimension ref="A3:A5"/>
+  <dimension ref="A3:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2014,9 +2011,14 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>165</v>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -2025,129 +2027,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7845C2-70F9-4E14-B1B5-A1C8583103A6}">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="25"/>
-    <col min="2" max="2" width="103.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="C7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="C8" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="C9" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>180</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62EBB9D9-62B1-4607-9165-74D788FDF57B}">
   <dimension ref="A2:B6"/>
   <sheetViews>
@@ -2187,12 +2066,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA56105-AB8B-4581-A967-BFD3464D4822}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2205,14 +2084,14 @@
       <c r="A1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="33"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
@@ -2342,7 +2221,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAA8839-6FCC-46CA-A458-98B76D0939D0}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -2411,7 +2290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F88F401-54DC-4AAA-BA84-9AC325020A6D}">
   <dimension ref="A2:A8"/>
   <sheetViews>
@@ -2451,7 +2330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06556CBD-FAF4-41D3-91F3-37168F04E350}">
   <dimension ref="A2:A4"/>
   <sheetViews>
@@ -2476,7 +2355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AFDD3F1-18CE-4FFB-B2C4-1CD7FECC91D7}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -2512,11 +2391,134 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7845C2-70F9-4E14-B1B5-A1C8583103A6}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="25"/>
+    <col min="2" max="2" width="103.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0118C388-E1CB-44F3-ACC3-F76C30052EB0}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2542,13 +2544,13 @@
         <v>159</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E1" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>200</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>201</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>156</v>
@@ -2563,7 +2565,7 @@
         <v>126</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>143</v>
@@ -2578,13 +2580,13 @@
         <v>93</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>133</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>44</v>
@@ -2616,19 +2618,19 @@
         <v>100</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>133</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>44</v>
@@ -2663,7 +2665,7 @@
         <v>160</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>133</v>
@@ -2692,11 +2694,11 @@
         <v>96</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>44</v>
@@ -2734,7 +2736,7 @@
         <v>160</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>133</v>
@@ -2769,17 +2771,17 @@
         <v>99</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>44</v>
@@ -2808,11 +2810,11 @@
         <v>101</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>44</v>
@@ -2836,7 +2838,7 @@
         <v>44</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -2850,7 +2852,7 @@
         <v>110</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>133</v>
@@ -2889,7 +2891,7 @@
         <v>162</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>44</v>
@@ -2930,7 +2932,7 @@
         <v>133</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>127</v>
@@ -2947,14 +2949,14 @@
       <c r="A12" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>110</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>110</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>44</v>
@@ -2978,7 +2980,7 @@
         <v>44</v>
       </c>
       <c r="L12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -2986,7 +2988,7 @@
         <v>30</v>
       </c>
       <c r="L13" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -3073,7 +3075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885D778B-E75C-4BF3-9FC1-547A1D09A614}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -3366,7 +3368,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
@@ -3397,7 +3399,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3512,7 +3514,7 @@
         <v>93</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -3520,7 +3522,7 @@
         <v>96</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -3528,7 +3530,7 @@
         <v>101</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3536,7 +3538,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3544,7 +3546,7 @@
         <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3732,22 +3734,22 @@
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update dod and tribe designation in pad
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PRJ\StateRx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BEF1B0-AC66-491F-8914-C6A6D99C0539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660FC9C2-EE94-449E-92B0-93C1E1AD4FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{25158DE5-819B-4E9C-8133-8EC91A336281}"/>
   </bookViews>
@@ -932,19 +932,19 @@
     <t xml:space="preserve">clean up the gis files, see list of files to delete in gis processing doc; also, delete files and code in R project associated w/ the old way of getting the pad info </t>
   </si>
   <si>
-    <t>Leaflet: add the ID number in the popup, adjust the zoom, republish w/ ag remove; make a google doc for feedback; put materials in participant folder;</t>
-  </si>
-  <si>
-    <t>PLOTS</t>
-  </si>
-  <si>
-    <t>add the west</t>
-  </si>
-  <si>
     <t>look into removing acres requested in AZ b/c they are unreliable; they are for emissions not rx fire tracking</t>
   </si>
   <si>
     <t xml:space="preserve">what data did I get from OR, does it include home owners burning piles? </t>
+  </si>
+  <si>
+    <t>do some qc between entity requesting and manager type from the pad</t>
+  </si>
+  <si>
+    <t>update gis documentation, processing steps to reflect final information</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> put materials in participant folder;</t>
   </si>
 </sst>
 </file>
@@ -1640,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8DF838-E91F-479B-BB7E-4DB4DA2419B3}">
-  <dimension ref="A1:P50"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1906,24 +1906,19 @@
         <v>252</v>
       </c>
     </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>256</v>
+      </c>
+    </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>245</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -2714,8 +2709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885D778B-E75C-4BF3-9FC1-547A1D09A614}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2744,7 +2739,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C3" s="3"/>
       <c r="K3" s="12" t="s">
@@ -3134,10 +3129,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C83686E-AC74-4D6B-A4E0-A59B79186090}">
-  <dimension ref="B2:Q62"/>
+  <dimension ref="B2:Q64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3372,7 +3367,12 @@
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>256</v>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UT and OR planned data
serious wrangaling, no success
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PRJ\StateRx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571BDB96-F07F-4E8A-A8D4-5F719CC5A8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BCE35B-7BE5-436D-BC2A-128144759CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3372" yWindow="1404" windowWidth="11892" windowHeight="12372" activeTab="3" xr2:uid="{25158DE5-819B-4E9C-8133-8EC91A336281}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{25158DE5-819B-4E9C-8133-8EC91A336281}"/>
   </bookViews>
   <sheets>
     <sheet name="state systems" sheetId="19" r:id="rId1"/>
     <sheet name="ToDoNow" sheetId="2" r:id="rId2"/>
-    <sheet name="ToDoLater" sheetId="18" r:id="rId3"/>
-    <sheet name="sit209" sheetId="20" r:id="rId4"/>
-    <sheet name="checklist" sheetId="12" r:id="rId5"/>
-    <sheet name="inquiries" sheetId="8" r:id="rId6"/>
-    <sheet name="burn status" sheetId="17" r:id="rId7"/>
-    <sheet name="plots" sheetId="3" r:id="rId8"/>
+    <sheet name="ca airdistrict contacts" sheetId="21" r:id="rId3"/>
+    <sheet name="ToDoLater" sheetId="18" r:id="rId4"/>
+    <sheet name="sit209" sheetId="20" r:id="rId5"/>
+    <sheet name="checklist" sheetId="12" r:id="rId6"/>
+    <sheet name="inquiries" sheetId="8" r:id="rId7"/>
+    <sheet name="burn status" sheetId="17" r:id="rId8"/>
+    <sheet name="plots" sheetId="3" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">checklist!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">checklist!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ToDoNow!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -111,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="254">
   <si>
     <t>after data are compiled draft check of the data to find and fix errors</t>
   </si>
@@ -583,9 +584,6 @@
     <t>Database improvements</t>
   </si>
   <si>
-    <t>OR planned data</t>
-  </si>
-  <si>
     <t>Remote sensing capabilities</t>
   </si>
   <si>
@@ -667,16 +665,10 @@
     <t>burn type keywords: consider adding "Prescribed Fire" to the list of broadcast burn words for classifying burn type; consider adding "slash" to the list of pile words for classifying burn type</t>
   </si>
   <si>
-    <t>clean up what is on nimbus and box files per T instructions</t>
-  </si>
-  <si>
     <t>figure out git ignore for StateRx repo gis files</t>
   </si>
   <si>
     <t>error check all pre processing scripts</t>
-  </si>
-  <si>
-    <t>review OR response and follow up questions</t>
   </si>
   <si>
     <t>geographic area of data collection (entire state, state and federal lands, etc)</t>
@@ -740,9 +732,6 @@
     <t>ID - follow up w/ ID airshed contact to get their data</t>
   </si>
   <si>
-    <t>MISC</t>
-  </si>
-  <si>
     <t>ASK T</t>
   </si>
   <si>
@@ -761,30 +750,18 @@
     <t>T priorities: figure out what the permitting process is for each state and data gaps</t>
   </si>
   <si>
-    <t>A - priority</t>
-  </si>
-  <si>
     <t>update gis documentation, processing steps to reflect final information and steps for pad and evt/lifeform</t>
   </si>
   <si>
-    <t>reporting of pile burns: priority? If so figure out how to best get consistent info</t>
-  </si>
-  <si>
     <t>update methods up to AFE</t>
   </si>
   <si>
     <t>spatial</t>
   </si>
   <si>
-    <t>move gis to remote desktop?</t>
-  </si>
-  <si>
     <t>add a minimal metadata to the gis files</t>
   </si>
   <si>
-    <t>emailed on 12/15</t>
-  </si>
-  <si>
     <t>analysis and pub: remote detction of rx fire</t>
   </si>
   <si>
@@ -834,6 +811,164 @@
   </si>
   <si>
     <t>ask Jim, does he know Kara (inrwin), can we call w/ her, invite T</t>
+  </si>
+  <si>
+    <t>consider removing the firefighter training burns from NV</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>Complete Data</t>
+  </si>
+  <si>
+    <t>Database improvements - DATE</t>
+  </si>
+  <si>
+    <t>ASK T - PILES</t>
+  </si>
+  <si>
+    <t>reporting of pile burns: priority? If so figure out how to best get consistent info; complete table of who records what and make suggestion</t>
+  </si>
+  <si>
+    <t>WA state - check how the date was figured; I tried to calculate the date by subtracting 1 year but I may need to account for burns that get a 2 year permit window</t>
+  </si>
+  <si>
+    <t>complete data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finish processing ID AMS data (remove status = draft; if status is proposed treat it as restricted); do I still use the IDL data? </t>
+  </si>
+  <si>
+    <t>South Coast</t>
+  </si>
+  <si>
+    <t>webinquiry@aqmd.gov</t>
+  </si>
+  <si>
+    <t>AIR DISTCIRCT</t>
+  </si>
+  <si>
+    <t>CONTACT</t>
+  </si>
+  <si>
+    <t>EMAILED</t>
+  </si>
+  <si>
+    <t>North Coast Unified</t>
+  </si>
+  <si>
+    <t>support@ncuaqmd.org</t>
+  </si>
+  <si>
+    <t>Northern Sierra</t>
+  </si>
+  <si>
+    <t>office@myairdistrict.com</t>
+  </si>
+  <si>
+    <t>sent trial email to 3 air districts</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>request submitted 1/16: https://onbase-pub.aqmd.gov/sAppNet/UnityForm.aspx?key=UFKey
+I called; they do permit open burning; submited a trial request to see what I get</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">consider trying to get point from the CA local air districts b/c reporting to pfirs is voluntary; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MAYBE TRY ASKING FOR THE SMOKE MANAGEMENT PLANS? An SMP is required for burns &gt;10 acres</t>
+    </r>
+  </si>
+  <si>
+    <t>emailed 1/18</t>
+  </si>
+  <si>
+    <t>make status for small burns in WA unknown</t>
+  </si>
+  <si>
+    <t>complete data, WA</t>
+  </si>
+  <si>
+    <t>complete data, UT</t>
+  </si>
+  <si>
+    <t>Complete Data, OR</t>
+  </si>
+  <si>
+    <t>database improvemnts</t>
+  </si>
+  <si>
+    <t>in make database script make sure that the date gets populated based on the new rules; update the date definition for the database as needed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">make a table documenting burn data info by state and figure out standardized processing 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>check processing in states that have 1 record per burn &amp; multiple dates; need to apply new logic in pre processing for these states</t>
+    </r>
+  </si>
+  <si>
+    <t>complete data, ID</t>
+  </si>
+  <si>
+    <t>review burn status classification; do it like ID</t>
+  </si>
+  <si>
+    <t>OR planned data (couldn't find a way to get info on planned acres per/unit so I didn't process)</t>
+  </si>
+  <si>
+    <t>complete data, MT</t>
+  </si>
+  <si>
+    <t>complete data, OR</t>
+  </si>
+  <si>
+    <t>review and maybe add Lane County data</t>
+  </si>
+  <si>
+    <t>try to standardize no burn reason to address the question why are burns not completed; what are the limitations; MT and ID, UT have a no burn reason, look at other states and make a table for who has what</t>
+  </si>
+  <si>
+    <t>complete data, CA</t>
+  </si>
+  <si>
+    <t>process the data from N coast district if feasible after call</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UT process all requests not just burn days; review ability to use requests; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>need help from T - see notes on Nimbus</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1004,7 +1139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1060,12 +1195,22 @@
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1468,7 +1613,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1481,74 +1626,74 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1559,10 +1704,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C83686E-AC74-4D6B-A4E0-A59B79186090}">
-  <dimension ref="A1:R62"/>
+  <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1576,35 +1721,38 @@
         <v>123</v>
       </c>
       <c r="B1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -1628,437 +1776,472 @@
         <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="B8" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>138</v>
+      <c r="B9" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>144</v>
-      </c>
-      <c r="C11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>195</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="C12" s="18" t="s">
+    <row r="11" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>195</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="N14" s="6"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="N15" s="6"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C16" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" t="s">
         <v>151</v>
       </c>
-      <c r="N16" s="6"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="N17" s="6"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>144</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>144</v>
-      </c>
-      <c r="C19" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>195</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>159</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>159</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>158</v>
       </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="C35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>158</v>
       </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>158</v>
       </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
         <v>158</v>
       </c>
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+      <c r="C38" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>158</v>
       </c>
-      <c r="C25" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>158</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>158</v>
-      </c>
-      <c r="C27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>158</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="C39" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="C41" s="38" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>161</v>
+      </c>
+      <c r="C42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C43" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B44" s="17" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>158</v>
-      </c>
-      <c r="C29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>158</v>
-      </c>
-      <c r="C30" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>158</v>
-      </c>
-      <c r="C31" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>158</v>
-      </c>
-      <c r="C32" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>160</v>
-      </c>
-      <c r="C33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>160</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>160</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>160</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>159</v>
-      </c>
-      <c r="C37" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>159</v>
-      </c>
-      <c r="C38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>159</v>
-      </c>
-      <c r="C39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>159</v>
-      </c>
-      <c r="C40" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>159</v>
-      </c>
-      <c r="C41" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>190</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>190</v>
-      </c>
-      <c r="C43" s="31" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="C44" s="33" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C44" s="35" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="C45" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>162</v>
-      </c>
-      <c r="C46" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="6"/>
       <c r="B47" t="s">
-        <v>144</v>
-      </c>
-      <c r="C47" s="31" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>206</v>
-      </c>
-      <c r="C48" t="s">
-        <v>207</v>
+        <v>137</v>
+      </c>
+      <c r="C47" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="1:4" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="6"/>
+      <c r="B49" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>220</v>
+      </c>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="6"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
+    <row r="50" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B50" s="43" t="s">
+        <v>244</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="6"/>
+      <c r="B51" s="36" t="s">
+        <v>221</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>250</v>
+      </c>
       <c r="D51" s="6"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
+      <c r="B52" s="42" t="s">
+        <v>239</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>253</v>
+      </c>
       <c r="D52" s="6"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="6"/>
+      <c r="B53" s="42" t="s">
+        <v>238</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>237</v>
+      </c>
       <c r="D53" s="6"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="6"/>
+      <c r="B54" s="42" t="s">
+        <v>241</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>242</v>
+      </c>
       <c r="D54" s="6"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="6"/>
+      <c r="B55" s="42" t="s">
+        <v>247</v>
+      </c>
+      <c r="C55" s="42" t="s">
+        <v>245</v>
+      </c>
       <c r="D55" s="6"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="6"/>
+      <c r="B56" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="C56" s="36" t="s">
+        <v>249</v>
+      </c>
       <c r="D56" s="6"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
-      <c r="B57" s="24"/>
-      <c r="C57" s="6"/>
+      <c r="B57" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>252</v>
+      </c>
       <c r="D57" s="6"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="10"/>
       <c r="D58" s="6"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="6"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="6"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="6"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="6"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="6"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="6"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{5C83686E-AC74-4D6B-A4E0-A59B79186090}">
@@ -2073,11 +2256,86 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71C587B-82EE-467E-9E7E-66A41BC360DC}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="41">
+        <v>45307</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" s="41">
+        <v>45307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" s="41">
+        <v>45307</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A7E7A33C-1186-4373-BF1B-2E83B7688A1A}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{BCE44AA2-7563-49E8-8F11-F17F4E3E731F}"/>
+    <hyperlink ref="B4" r:id="rId3" display="mailto:office@myairdistrict.com" xr:uid="{24F7056A-C9B4-4F31-A62D-6BF51FFB6C6C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A5E718-D21A-4D29-AD6C-7AF1EFCBAE25}">
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2092,33 +2350,33 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2128,15 +2386,15 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2145,28 +2403,31 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>146</v>
+      <c r="A15" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B19" t="s">
         <v>131</v>
@@ -2174,7 +2435,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -2182,7 +2443,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
@@ -2190,7 +2451,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
@@ -2201,44 +2462,44 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F1F03B5-0252-4B3D-A5BE-D7FE39D465EB}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
-        <v>210</v>
+      <c r="A1" s="33" t="s">
+        <v>202</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
-        <v>212</v>
+      <c r="A2" s="33" t="s">
+        <v>204</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
-        <v>214</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>215</v>
+      <c r="A3" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>207</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -2252,7 +2513,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D5" s="4" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -2260,7 +2521,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D6" s="4" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -2268,7 +2529,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D7" s="4" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -2282,7 +2543,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -2296,12 +2557,12 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -2313,7 +2574,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0118C388-E1CB-44F3-ACC3-F76C30052EB0}">
   <dimension ref="A1:O27"/>
   <sheetViews>
@@ -2907,7 +3168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7D9BAF-C83F-4253-8659-5711E6B968C9}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -2965,7 +3226,7 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2981,7 +3242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7845C2-70F9-4E14-B1B5-A1C8583103A6}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -3104,7 +3365,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA56105-AB8B-4581-A967-BFD3464D4822}">
   <dimension ref="A1:I25"/>
   <sheetViews>
@@ -3127,10 +3388,10 @@
       <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
@@ -3208,7 +3469,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
@@ -3216,7 +3477,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
@@ -3224,7 +3485,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
@@ -3232,7 +3493,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B23" t="s">
         <v>27</v>
@@ -3240,7 +3501,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B24" t="s">
         <v>28</v>
@@ -3248,7 +3509,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B25" t="s">
         <v>31</v>

</xml_diff>